<commit_message>
documenting more test cases, final updates to the readme file
</commit_message>
<xml_diff>
--- a/Performace-testing-results.xlsx
+++ b/Performace-testing-results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nodes</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t xml:space="preserve">total time patients waited</t>
+  </si>
+  <si>
+    <t>ambulances</t>
+  </si>
+  <si>
+    <t>patients</t>
   </si>
 </sst>
 </file>
@@ -59,8 +65,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,7 +114,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -147,7 +156,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -170,7 +179,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -194,6 +203,14 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:axId val="2140841507"/>
         <c:axId val="2140841508"/>
       </c:scatterChart>
@@ -308,6 +325,7 @@
         </c:txPr>
         <c:crossAx val="2140841508"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2140841508"/>
@@ -441,8 +459,8 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="400049" y="1441449"/>
-      <a:ext cx="4552949" cy="2724149"/>
+      <a:off x="1009648" y="1441449"/>
+      <a:ext cx="4895849" cy="2724149"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
       <a:avLst/>
@@ -511,7 +529,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -553,7 +571,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$6</c:f>
+              <c:f>Sheet1!$B$2:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -576,7 +594,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -600,6 +618,14 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:dLbls>
+          <c:showBubbleSize val="0"/>
+          <c:showCatName val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showPercent val="0"/>
+          <c:showSerName val="0"/>
+          <c:showVal val="0"/>
+        </c:dLbls>
         <c:axId val="2140841505"/>
         <c:axId val="2140841506"/>
       </c:scatterChart>
@@ -695,6 +721,7 @@
         </c:txPr>
         <c:crossAx val="2140841506"/>
         <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="2140841506"/>
@@ -809,7 +836,623 @@
   </c:chart>
   <c:spPr bwMode="auto">
     <a:xfrm>
-      <a:off x="5724524" y="1441449"/>
+      <a:off x="6677023" y="1441449"/>
+      <a:ext cx="4552949" cy="2724149"/>
+    </a:xfrm>
+    <a:prstGeom prst="rect">
+      <a:avLst/>
+    </a:prstGeom>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total distance travelled</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9811.004593468691</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9432.354936168373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6658.987890601285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="2140841551"/>
+        <c:axId val="2140841552"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2140841551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.000000"/>
+          <c:min val="1.000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr bwMode="auto">
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140841552"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2140841552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Total Distance Travelled</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr bwMode="auto">
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140841551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr bwMode="auto">
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr bwMode="auto">
+    <a:xfrm>
+      <a:off x="733424" y="5505449"/>
+      <a:ext cx="4552949" cy="2724149"/>
+    </a:xfrm>
+    <a:prstGeom prst="rect">
+      <a:avLst/>
+    </a:prstGeom>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins l="0.69999999999999996" r="0.69999999999999996" t="0.75" b="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total time patients waited</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr bwMode="auto">
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$27:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="2140841553"/>
+        <c:axId val="2140841554"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2140841553"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3.000000"/>
+          <c:min val="1.000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr bwMode="auto">
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140841554"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2140841554"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr bwMode="auto">
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr/>
+                  <a:t>Total Time Patients Waited</a:t>
+                </a:r>
+                <a:endParaRPr/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr bwMode="auto">
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2140841553"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr bwMode="auto">
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr bwMode="auto">
+    <a:xfrm>
+      <a:off x="5676899" y="5505449"/>
       <a:ext cx="4552949" cy="2724149"/>
     </a:xfrm>
     <a:prstGeom prst="rect">
@@ -932,6 +1575,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1478,6 +2201,1096 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" spc="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" spc="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr bwMode="auto">
+      <a:prstGeom prst="rect">
+        <a:avLst/>
+      </a:prstGeom>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2026,16 +3839,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400048</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>19048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>463549</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>463548</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>76198</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2045,8 +3858,8 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="400049" y="1441449"/>
-        <a:ext cx="4552949" cy="2724149"/>
+        <a:off x="1009648" y="1441449"/>
+        <a:ext cx="4895849" cy="2724149"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2058,16 +3871,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>15874</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>15873</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>19048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>301624</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>301623</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:rowOff>76198</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2077,12 +3890,76 @@
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5724524" y="1441449"/>
+        <a:off x="6677023" y="1441449"/>
         <a:ext cx="4552949" cy="2724149"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>549274</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="753606581" name=""/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="733424" y="5505449"/>
+        <a:ext cx="4552949" cy="2724149"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330199</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6349</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1465866125" name=""/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5676899" y="5505449"/>
+        <a:ext cx="4552949" cy="2724149"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2584,81 +4461,138 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="5.97265625"/>
-    <col bestFit="1" min="2" max="2" width="20.25390625"/>
-    <col bestFit="1" min="3" max="3" width="22.7734375"/>
+    <col bestFit="1" min="1" max="1" width="11.19140625"/>
+    <col bestFit="1" min="2" max="2" width="7.76171875"/>
+    <col bestFit="1" min="3" max="3" width="20.25390625"/>
+    <col bestFit="1" min="4" max="4" width="22.7734375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2">
+      <c r="B2">
         <v>10</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>135.78657069713842</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>18</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3">
+      <c r="B3">
         <v>25</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>383.60155539481292</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>27</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4">
+      <c r="B4">
         <v>50</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>849.43464125825835</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>27</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5">
+      <c r="B5">
         <v>75</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2118.0385402182719</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>35</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6">
+      <c r="B6">
         <v>100</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>2756.7386558677786</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>39</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>9811.0045934686914</v>
+      </c>
+      <c r="D27">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>9432.3549361683727</v>
+      </c>
+      <c r="D28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>6658.9878906012846</v>
+      </c>
+      <c r="D29">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>